<commit_message>
edit to excel spreadsheet to mark completted articles (green), articles in process (yellow), articles assigned or in need of review (red). Also started new column for whether the article is attributed to Nelson or not
</commit_message>
<xml_diff>
--- a/ResearchDevelopment/FileCorrelation-ForVersioning.xlsx
+++ b/ResearchDevelopment/FileCorrelation-ForVersioning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Becca\Documents\GitHub\CitySlaveGirls-ChicagoDailyTimes1888\ResearchDevelopment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nas\Documents\GitHub\CitySlaveGirls\ResearchDevelopment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>Barkley - The White Slave Girls of Chicago</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t>WSGC01 WSGC02 WSGC03</t>
+  </si>
+  <si>
+    <t>not Nell</t>
   </si>
 </sst>
 </file>
@@ -348,12 +351,30 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -368,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -381,6 +402,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -665,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,10 +730,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -705,10 +744,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -719,18 +758,18 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -741,10 +780,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -755,10 +794,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -805,10 +844,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -819,10 +858,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -833,10 +872,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -844,6 +883,9 @@
       </c>
       <c r="D13" s="2" t="s">
         <v>81</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -861,10 +903,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="8" t="s">
         <v>96</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -897,10 +939,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -919,10 +961,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -947,10 +989,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1017,10 +1059,10 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="9" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edits to 1888-08-10 transcription and coding, adding to Site Index, edits to excel spreadsheet
</commit_message>
<xml_diff>
--- a/ResearchDevelopment/FileCorrelation-ForVersioning.xlsx
+++ b/ResearchDevelopment/FileCorrelation-ForVersioning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>Barkley - The White Slave Girls of Chicago</t>
   </si>
@@ -329,7 +329,10 @@
     <t>WSGC01 WSGC02 WSGC03</t>
   </si>
   <si>
-    <t>not Nell</t>
+    <t>Is Nell the reporter?</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -389,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -421,6 +424,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +720,7 @@
     <col min="2" max="2" width="61" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -722,8 +728,12 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -884,8 +894,8 @@
       <c r="D13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>101</v>
+      <c r="E13" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1097,6 +1107,9 @@
       <c r="A37" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
finished transcription and initial coding of  1888-08-10
</commit_message>
<xml_diff>
--- a/ResearchDevelopment/FileCorrelation-ForVersioning.xlsx
+++ b/ResearchDevelopment/FileCorrelation-ForVersioning.xlsx
@@ -339,7 +339,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +348,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF183691"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color rgb="FF183691"/>
       <name val="Consolas"/>
@@ -380,7 +395,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -388,11 +403,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -427,6 +457,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -710,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +1020,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>53</v>
       </c>
@@ -998,11 +1034,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="13" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1111,6 +1147,6 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor update to file correlation spreadsheet to account for articles added to site but still need proofed
</commit_message>
<xml_diff>
--- a/ResearchDevelopment/FileCorrelation-ForVersioning.xlsx
+++ b/ResearchDevelopment/FileCorrelation-ForVersioning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nas\Documents\GitHub\CitySlaveGirls\ResearchDevelopment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rebecca Parker\Documents\GitHub\CitySlaveGirls\ResearchDevelopment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -338,7 +338,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -455,14 +455,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,10 +764,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="12"/>
+      <c r="D1" s="14"/>
       <c r="E1" s="1" t="s">
         <v>101</v>
       </c>
@@ -890,10 +890,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1035,10 +1035,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="3" t="s">

</xml_diff>

<commit_message>
adding new CSG with more complete series (includes letters to editor, additional related articles, and editorial pieces related to the CSG series) - These are all from the actual Chicago Times Newspaper series (not reprints)
</commit_message>
<xml_diff>
--- a/ResearchDevelopment/FileCorrelation-ForVersioning.xlsx
+++ b/ResearchDevelopment/FileCorrelation-ForVersioning.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="422">
   <si>
     <t>Barkley - The White Slave Girls of Chicago</t>
   </si>
@@ -379,9 +379,6 @@
     <t>CT001_P2</t>
   </si>
   <si>
-    <t>CT001_A4</t>
-  </si>
-  <si>
     <t>CT002_P1</t>
   </si>
   <si>
@@ -457,9 +454,6 @@
     <t>Degrading Female Labor</t>
   </si>
   <si>
-    <t>CT003_U1</t>
-  </si>
-  <si>
     <t>Snippets of text mentioning Never-Rip Libel Lawsuit against the paper</t>
   </si>
   <si>
@@ -1286,6 +1280,18 @@
   </si>
   <si>
     <t>1888-08-06</t>
+  </si>
+  <si>
+    <t>CT002_O2</t>
+  </si>
+  <si>
+    <t>Concentrating Wealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> My first impulse was for revenge, but remembering that I was a poor girl looking for work I contented myself by petting my damaged left knee and right elbow.</t>
+  </si>
+  <si>
+    <t>lot's of linking prostitution</t>
   </si>
 </sst>
 </file>
@@ -2208,10 +2214,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J84"/>
+  <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2234,7 +2240,7 @@
         <v>106</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>107</v>
@@ -2291,7 +2297,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E4" s="19" t="s">
         <v>98</v>
@@ -2308,7 +2314,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E5" s="19" t="s">
         <v>98</v>
@@ -2316,7 +2322,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B6" s="19">
         <v>4</v>
@@ -2325,7 +2331,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>98</v>
@@ -2333,7 +2339,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B7" s="19">
         <v>8</v>
@@ -2350,7 +2356,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8" s="19">
         <v>1</v>
@@ -2359,7 +2365,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>98</v>
@@ -2367,7 +2373,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" s="19">
         <v>2</v>
@@ -2376,7 +2382,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>98</v>
@@ -2384,7 +2390,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B10" s="19">
         <v>4</v>
@@ -2393,7 +2399,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>98</v>
@@ -2401,7 +2407,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" s="19">
         <v>4</v>
@@ -2410,18 +2416,18 @@
         <v>4</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>129</v>
+        <v>418</v>
       </c>
       <c r="B12" s="19">
         <v>4</v>
@@ -2436,21 +2442,12 @@
         <v>98</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="I12" s="25" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B13" s="19">
         <v>4</v>
@@ -2459,51 +2456,63 @@
         <v>4</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F13" s="20"/>
+      <c r="F13" s="20" t="s">
+        <v>133</v>
+      </c>
       <c r="G13" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="H13" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="I13" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="I13" s="25" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B14" s="19">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="E14" s="19" t="s">
         <v>98</v>
+      </c>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B15" s="19">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>98</v>
@@ -2511,33 +2520,36 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B16" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>98</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B17" s="19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>98</v>
@@ -2545,7 +2557,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B18" s="19">
         <v>4</v>
@@ -2554,18 +2566,15 @@
         <v>5</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B19" s="19">
         <v>4</v>
@@ -2574,21 +2583,21 @@
         <v>5</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="I19" s="25" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="B20" s="19">
         <v>4</v>
@@ -2597,53 +2606,59 @@
         <v>5</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>130</v>
+        <v>218</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="I20" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="J20" s="20" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>151</v>
-      </c>
       <c r="B21" s="19">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>98</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="I21" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B22" s="19">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>98</v>
@@ -2651,24 +2666,24 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B23" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B24" s="19">
         <v>2</v>
@@ -2677,38 +2692,38 @@
         <v>6</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="I24" s="24" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B25" s="19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="F25" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="I25" s="24" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B26" s="19">
         <v>4</v>
@@ -2717,47 +2732,47 @@
         <v>6</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F26" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="I26" s="24" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B27" s="19">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="E27" s="19" t="s">
         <v>98</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="I27" s="24" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B28" s="19">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="E28" s="19" t="s">
         <v>98</v>
@@ -2765,24 +2780,24 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B29" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E29" s="19" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B30" s="19">
         <v>2</v>
@@ -2791,27 +2806,15 @@
         <v>7</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E30" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F30" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="G30" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="H30" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="I30" s="24" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B31" s="19">
         <v>2</v>
@@ -2820,27 +2823,27 @@
         <v>7</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E31" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="H31" s="21" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="I31" s="24" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B32" s="19">
         <v>2</v>
@@ -2849,27 +2852,27 @@
         <v>7</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="I32" s="24" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B33" s="19">
         <v>2</v>
@@ -2878,27 +2881,27 @@
         <v>7</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E33" s="19" t="s">
         <v>99</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="G33" s="21" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I33" s="24" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B34" s="19">
         <v>2</v>
@@ -2907,27 +2910,27 @@
         <v>7</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>99</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="G34" s="21" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="H34" s="21" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="I34" s="24" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B35" s="19">
         <v>2</v>
@@ -2936,27 +2939,27 @@
         <v>7</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G35" s="21" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="H35" s="21" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="I35" s="24" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B36" s="19">
         <v>2</v>
@@ -2965,27 +2968,27 @@
         <v>7</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E36" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="G36" s="21" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="I36" s="24" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B37" s="19">
         <v>2</v>
@@ -2994,27 +2997,27 @@
         <v>7</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E37" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G37" s="21" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="H37" s="21" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I37" s="24" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B38" s="19">
         <v>2</v>
@@ -3023,24 +3026,27 @@
         <v>7</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>199</v>
+        <v>196</v>
+      </c>
+      <c r="G38" s="21" t="s">
+        <v>163</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I38" s="24" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="B39" s="19">
         <v>2</v>
@@ -3049,27 +3055,24 @@
         <v>7</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="G39" s="22" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="H39" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="I39" s="24" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="18" t="s">
         <v>205</v>
-      </c>
-      <c r="I39" s="24" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
-        <v>208</v>
       </c>
       <c r="B40" s="19">
         <v>2</v>
@@ -3078,21 +3081,27 @@
         <v>7</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E40" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>209</v>
+        <v>204</v>
+      </c>
+      <c r="G40" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="H40" s="21" t="s">
+        <v>203</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B41" s="19">
         <v>2</v>
@@ -3101,44 +3110,44 @@
         <v>7</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E41" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="I41" s="24" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="300" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B42" s="19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E42" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I42" s="24" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="300" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B43" s="19">
         <v>4</v>
@@ -3147,47 +3156,53 @@
         <v>7</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="E43" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B44" s="19">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>114</v>
+        <v>218</v>
       </c>
       <c r="E44" s="19" t="s">
         <v>98</v>
+      </c>
+      <c r="F44" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="I44" s="24" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B45" s="19">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="E45" s="19" t="s">
         <v>98</v>
@@ -3195,24 +3210,24 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B46" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B47" s="19">
         <v>2</v>
@@ -3221,47 +3236,44 @@
         <v>8</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E47" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F47" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="G47" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="H47" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="I47" s="24" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B48" s="19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="E48" s="19" t="s">
         <v>98</v>
       </c>
+      <c r="F48" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="G48" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="H48" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="I48" s="24" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B49" s="19">
         <v>4</v>
@@ -3270,21 +3282,18 @@
         <v>8</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="E49" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F49" s="21" t="s">
-        <v>232</v>
-      </c>
       <c r="I49" s="24" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B50" s="19">
         <v>4</v>
@@ -3293,44 +3302,50 @@
         <v>8</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="E50" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B51" s="19">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>114</v>
+        <v>218</v>
       </c>
       <c r="E51" s="19" t="s">
         <v>98</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="I51" s="24" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B52" s="19">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D52" s="21" t="s">
         <v>114</v>
@@ -3339,32 +3354,26 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B53" s="19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>9</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="E53" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F53" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="I53" s="24" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B54" s="19">
         <v>4</v>
@@ -3373,38 +3382,44 @@
         <v>9</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="E54" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="I54" s="24" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B55" s="19">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>9</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>127</v>
+        <v>218</v>
       </c>
       <c r="E55" s="19" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="F55" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="I55" s="24" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B56" s="19">
         <v>17</v>
@@ -3413,27 +3428,15 @@
         <v>9</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E56" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F56" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="G56" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="H56" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="I56" s="24" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B57" s="19">
         <v>17</v>
@@ -3442,27 +3445,27 @@
         <v>9</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E57" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G57" s="21" t="s">
-        <v>251</v>
+        <v>224</v>
       </c>
       <c r="H57" s="21" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="I57" s="24" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B58" s="19">
         <v>17</v>
@@ -3471,27 +3474,27 @@
         <v>9</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E58" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F58" s="21" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="G58" s="21" t="s">
-        <v>165</v>
+        <v>249</v>
       </c>
       <c r="H58" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="I58" s="24" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
         <v>255</v>
-      </c>
-      <c r="I58" s="24" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="18" t="s">
-        <v>258</v>
       </c>
       <c r="B59" s="19">
         <v>17</v>
@@ -3500,27 +3503,27 @@
         <v>9</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E59" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F59" s="21" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="G59" s="21" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="H59" s="21" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="I59" s="24" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B60" s="19">
         <v>17</v>
@@ -3529,27 +3532,27 @@
         <v>9</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E60" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F60" s="21" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G60" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="H60" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="I60" s="24" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
         <v>263</v>
-      </c>
-      <c r="H60" s="21" t="s">
-        <v>267</v>
-      </c>
-      <c r="I60" s="24" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A61" s="18" t="s">
-        <v>268</v>
       </c>
       <c r="B61" s="19">
         <v>17</v>
@@ -3558,27 +3561,27 @@
         <v>9</v>
       </c>
       <c r="D61" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E61" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F61" s="21" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="G61" s="21" t="s">
-        <v>226</v>
+        <v>261</v>
       </c>
       <c r="H61" s="21" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="I61" s="24" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B62" s="19">
         <v>17</v>
@@ -3587,27 +3590,27 @@
         <v>9</v>
       </c>
       <c r="D62" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E62" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F62" s="21" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="G62" s="21" t="s">
-        <v>274</v>
+        <v>224</v>
       </c>
       <c r="H62" s="21" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="B63" s="19">
         <v>17</v>
@@ -3616,27 +3619,27 @@
         <v>9</v>
       </c>
       <c r="D63" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E63" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F63" s="21" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="G63" s="21" t="s">
-        <v>226</v>
+        <v>272</v>
       </c>
       <c r="H63" s="21" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="I63" s="24" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B64" s="19">
         <v>17</v>
@@ -3645,27 +3648,27 @@
         <v>9</v>
       </c>
       <c r="D64" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E64" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="G64" s="21" t="s">
-        <v>263</v>
+        <v>224</v>
       </c>
       <c r="H64" s="21" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="I64" s="24" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B65" s="19">
         <v>17</v>
@@ -3674,27 +3677,27 @@
         <v>9</v>
       </c>
       <c r="D65" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E65" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F65" s="21" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="G65" s="21" t="s">
-        <v>226</v>
+        <v>261</v>
       </c>
       <c r="H65" s="21" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B66" s="19">
         <v>17</v>
@@ -3703,27 +3706,27 @@
         <v>9</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E66" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F66" s="21" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="G66" s="21" t="s">
-        <v>290</v>
+        <v>224</v>
       </c>
       <c r="H66" s="21" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="I66" s="24" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B67" s="19">
         <v>17</v>
@@ -3732,27 +3735,27 @@
         <v>9</v>
       </c>
       <c r="D67" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E67" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F67" s="21" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="G67" s="21" t="s">
-        <v>263</v>
+        <v>288</v>
       </c>
       <c r="H67" s="21" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="I67" s="24" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B68" s="19">
         <v>17</v>
@@ -3761,27 +3764,27 @@
         <v>9</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E68" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F68" s="21" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="G68" s="21" t="s">
-        <v>226</v>
+        <v>261</v>
       </c>
       <c r="H68" s="21" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="I68" s="24" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="B69" s="19">
         <v>17</v>
@@ -3790,27 +3793,27 @@
         <v>9</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E69" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F69" s="21" t="s">
-        <v>169</v>
+        <v>296</v>
       </c>
       <c r="G69" s="21" t="s">
-        <v>263</v>
+        <v>224</v>
       </c>
       <c r="H69" s="21" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="I69" s="24" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B70" s="19">
         <v>17</v>
@@ -3819,27 +3822,27 @@
         <v>9</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E70" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F70" s="21" t="s">
-        <v>305</v>
+        <v>167</v>
       </c>
       <c r="G70" s="21" t="s">
-        <v>226</v>
+        <v>261</v>
       </c>
       <c r="H70" s="21" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="I70" s="24" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B71" s="19">
         <v>17</v>
@@ -3848,27 +3851,27 @@
         <v>9</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E71" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F71" s="21" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="G71" s="21" t="s">
-        <v>183</v>
+        <v>224</v>
       </c>
       <c r="H71" s="21" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="I71" s="24" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="B72" s="19">
         <v>17</v>
@@ -3877,27 +3880,27 @@
         <v>9</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E72" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F72" s="21" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="G72" s="21" t="s">
-        <v>226</v>
+        <v>181</v>
       </c>
       <c r="H72" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="I72" s="24" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="B73" s="19">
         <v>17</v>
@@ -3906,27 +3909,27 @@
         <v>9</v>
       </c>
       <c r="D73" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E73" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F73" s="21" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G73" s="21" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H73" s="21" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I73" s="24" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B74" s="19">
         <v>17</v>
@@ -3935,27 +3938,27 @@
         <v>9</v>
       </c>
       <c r="D74" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E74" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F74" s="21" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G74" s="21" t="s">
-        <v>263</v>
+        <v>224</v>
       </c>
       <c r="H74" s="21" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="I74" s="24" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B75" s="19">
         <v>17</v>
@@ -3964,27 +3967,27 @@
         <v>9</v>
       </c>
       <c r="D75" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E75" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F75" s="21" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="G75" s="21" t="s">
-        <v>226</v>
+        <v>261</v>
       </c>
       <c r="H75" s="21" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="I75" s="24" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="B76" s="19">
         <v>17</v>
@@ -3993,215 +3996,244 @@
         <v>9</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E76" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F76" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="G76" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="H76" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="I76" s="24" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="B77" s="19">
+        <v>17</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E77" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F77" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="G77" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="H77" s="21" t="s">
+        <v>328</v>
+      </c>
+      <c r="I77" s="24" t="s">
         <v>329</v>
-      </c>
-      <c r="G76" s="21" t="s">
-        <v>263</v>
-      </c>
-      <c r="H76" s="21" t="s">
-        <v>330</v>
-      </c>
-      <c r="I76" s="24" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="18" t="s">
-        <v>332</v>
-      </c>
-      <c r="B77" s="19">
-        <v>1</v>
-      </c>
-      <c r="C77" s="18" t="s">
-        <v>419</v>
-      </c>
-      <c r="D77" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="E77" s="19" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B78" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D78" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E78" s="19" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B79" s="19">
         <v>2</v>
       </c>
       <c r="C79" s="18" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D79" s="21" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E79" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F79" s="21" t="s">
-        <v>335</v>
-      </c>
-      <c r="G79" s="21" t="s">
-        <v>336</v>
-      </c>
-      <c r="H79" s="21" t="s">
-        <v>337</v>
-      </c>
-      <c r="I79" s="24" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="B80" s="19">
         <v>2</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D80" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E80" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F80" s="21" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="G80" s="21" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="H80" s="21" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="I80" s="24" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="B81" s="19">
         <v>2</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D81" s="21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E81" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F81" s="21" t="s">
-        <v>345</v>
+        <v>338</v>
+      </c>
+      <c r="G81" s="21" t="s">
+        <v>339</v>
       </c>
       <c r="H81" s="21" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="I81" s="24" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="B82" s="19">
         <v>2</v>
       </c>
       <c r="C82" s="18" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D82" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E82" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F82" s="21" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="H82" s="21" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="I82" s="24" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A83" s="18" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="B83" s="19">
         <v>2</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D83" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E83" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F83" s="21" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="H83" s="21" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="I83" s="24" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="18" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="B84" s="19">
         <v>2</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D84" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E84" s="19" t="s">
         <v>98</v>
       </c>
       <c r="F84" s="21" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="H84" s="21" t="s">
-        <v>358</v>
+        <v>352</v>
+      </c>
+      <c r="I84" s="24" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A85" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="B85" s="19">
+        <v>2</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>417</v>
+      </c>
+      <c r="D85" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E85" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F85" s="21" t="s">
+        <v>355</v>
+      </c>
+      <c r="H85" s="21" t="s">
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -4233,109 +4265,109 @@
         <v>3</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" s="27" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="27" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="C5" s="27" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" s="27" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C9" s="27" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="C10" s="27" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="C11" s="27" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="C12" s="27" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" s="27" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="C14" s="27" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="C15" s="27" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="C16" s="27" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="C17" s="27" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="C18" s="27" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4346,76 +4378,76 @@
         <v>114</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C22" s="27" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>382</v>
+      </c>
+      <c r="B23" t="s">
+        <v>383</v>
+      </c>
+      <c r="C23" s="27" t="s">
         <v>384</v>
-      </c>
-      <c r="B23" t="s">
-        <v>385</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="C24" s="27" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="C25" s="27" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C26" s="27" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="C27" s="27" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" s="27" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="C29" s="27" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="C30" s="27" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="C31" s="27" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C33" s="27" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4426,7 +4458,7 @@
         <v>114</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4434,100 +4466,100 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="C36" s="27" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="C37" s="27" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="C38" s="27" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C39" s="27" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C40" s="27" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C41" s="27" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="C42" s="27" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C43" s="27" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C44" s="27" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="C45" s="27" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C46" s="27" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="C47" s="27" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C48" s="27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="27" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="51" spans="3:3" ht="75" x14ac:dyDescent="0.25">
       <c r="C51" s="27" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="52" spans="3:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C52" s="27" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="53" spans="3:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C53" s="27" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="54" spans="3:3" ht="120" x14ac:dyDescent="0.25">
       <c r="C54" s="27" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more of the revised articles from CSG series including additional articles, letters to editor, etc.
</commit_message>
<xml_diff>
--- a/ResearchDevelopment/FileCorrelation-ForVersioning.xlsx
+++ b/ResearchDevelopment/FileCorrelation-ForVersioning.xlsx
@@ -2216,8 +2216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2269,7 +2269,7 @@
         <v>114</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2283,7 +2283,7 @@
         <v>114</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding notes on scan quality
</commit_message>
<xml_diff>
--- a/ResearchDevelopment/FileCorrelation-ForVersioning.xlsx
+++ b/ResearchDevelopment/FileCorrelation-ForVersioning.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="423">
   <si>
     <t>Barkley - The White Slave Girls of Chicago</t>
   </si>
@@ -1292,6 +1292,9 @@
   </si>
   <si>
     <t>lot's of linking prostitution</t>
+  </si>
+  <si>
+    <t>Told in the Pulpit.</t>
   </si>
 </sst>
 </file>
@@ -2214,10 +2217,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="B83" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4234,6 +4237,51 @@
       </c>
       <c r="H85" s="21" t="s">
         <v>356</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="19">
+        <v>8</v>
+      </c>
+      <c r="C86" s="18" t="s">
+        <v>417</v>
+      </c>
+      <c r="D86" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E86" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F86" s="21" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B87" s="19">
+        <v>1</v>
+      </c>
+      <c r="C87" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D87" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E87" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B88" s="19">
+        <v>2</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D88" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E88" s="19" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>